<commit_message>
adding updated input.xlsx file
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Sr No</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Sanjeev</t>
+  </si>
+  <si>
+    <t>Birender</t>
+  </si>
+  <si>
+    <t>Govinda</t>
   </si>
 </sst>
 </file>
@@ -368,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -429,6 +435,28 @@
       </c>
       <c r="C5">
         <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>980</v>
       </c>
     </row>
   </sheetData>

</xml_diff>